<commit_message>
Integrated report generation and appending to report in main()
</commit_message>
<xml_diff>
--- a/tests/SOLUSDT_analysis.xlsx
+++ b/tests/SOLUSDT_analysis.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Data" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Price Analysis" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Technical Analysis" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Fundamental Analysis" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sentiment Analysis" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Predictions" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Dashboard" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Price Analysis" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Technical Analysis" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Fundamental Analysis" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Sentiment Analysis" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Predictions" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -167,14 +167,14 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -197,26 +197,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$23</f>
+              <f>'Price Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$C$4:$C$23</f>
+              <f>'Price Analysis'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -229,26 +229,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$23</f>
+              <f>'Price Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$D$4:$D$23</f>
+              <f>'Price Analysis'!$D$4:$D$24</f>
             </numRef>
           </val>
         </ser>
@@ -261,26 +261,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$23</f>
+              <f>'Price Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$E$4:$E$23</f>
+              <f>'Price Analysis'!$E$4:$E$24</f>
             </numRef>
           </val>
         </ser>
@@ -296,8 +296,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -323,8 +323,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -350,14 +350,14 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <style val="10"/>
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -381,18 +381,18 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$23</f>
+              <f>'Price Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$H$4:$H$23</f>
+              <f>'Price Analysis'!$H$4:$H$24</f>
             </numRef>
           </val>
         </ser>
@@ -421,8 +421,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -448,13 +448,13 @@
 </file>
 
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -477,26 +477,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$23</f>
+              <f>'Technical Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$E$4:$E$23</f>
+              <f>'Technical Analysis'!$E$4:$E$24</f>
             </numRef>
           </val>
         </ser>
@@ -524,8 +524,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -551,13 +551,13 @@
 </file>
 
 <file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -580,26 +580,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$23</f>
+              <f>'Technical Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$C$4:$C$23</f>
+              <f>'Technical Analysis'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -612,26 +612,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$23</f>
+              <f>'Technical Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$D$4:$D$23</f>
+              <f>'Technical Analysis'!$D$4:$D$24</f>
             </numRef>
           </val>
         </ser>
@@ -659,8 +659,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -686,13 +686,13 @@
 </file>
 
 <file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -715,26 +715,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$23</f>
+              <f>'Fundamental Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$C$4:$C$23</f>
+              <f>'Fundamental Analysis'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -747,26 +747,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$23</f>
+              <f>'Fundamental Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$D$4:$D$23</f>
+              <f>'Fundamental Analysis'!$D$4:$D$24</f>
             </numRef>
           </val>
         </ser>
@@ -779,26 +779,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$23</f>
+              <f>'Fundamental Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$E$4:$E$23</f>
+              <f>'Fundamental Analysis'!$E$4:$E$24</f>
             </numRef>
           </val>
         </ser>
@@ -811,26 +811,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$23</f>
+              <f>'Fundamental Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$F$4:$F$23</f>
+              <f>'Fundamental Analysis'!$F$4:$F$24</f>
             </numRef>
           </val>
         </ser>
@@ -843,26 +843,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$23</f>
+              <f>'Fundamental Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$G$4:$G$23</f>
+              <f>'Fundamental Analysis'!$G$4:$G$24</f>
             </numRef>
           </val>
         </ser>
@@ -890,8 +890,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -917,13 +917,13 @@
 </file>
 
 <file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -946,26 +946,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$23</f>
+              <f>'Sentiment Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$C$4:$C$23</f>
+              <f>'Sentiment Analysis'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -978,26 +978,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$23</f>
+              <f>'Sentiment Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$D$4:$D$23</f>
+              <f>'Sentiment Analysis'!$D$4:$D$24</f>
             </numRef>
           </val>
         </ser>
@@ -1010,26 +1010,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$23</f>
+              <f>'Sentiment Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$E$4:$E$23</f>
+              <f>'Sentiment Analysis'!$E$4:$E$24</f>
             </numRef>
           </val>
         </ser>
@@ -1057,8 +1057,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -1084,13 +1084,13 @@
 </file>
 
 <file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1113,26 +1113,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$23</f>
+              <f>'Sentiment Analysis'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$F$4:$F$23</f>
+              <f>'Sentiment Analysis'!$F$4:$F$24</f>
             </numRef>
           </val>
         </ser>
@@ -1160,8 +1160,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -1187,13 +1187,13 @@
 </file>
 
 <file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1216,26 +1216,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$23</f>
+              <f>'Predictions'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$23</f>
+              <f>'Predictions'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -1248,26 +1248,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$23</f>
+              <f>'Predictions'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$D$4:$D$23</f>
+              <f>'Predictions'!$D$4:$D$24</f>
             </numRef>
           </val>
         </ser>
@@ -1295,8 +1295,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -1322,13 +1322,13 @@
 </file>
 
 <file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
-<chartSpace xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
+<chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns="http://schemas.openxmlformats.org/drawingml/2006/chart">
   <chart>
     <title>
       <tx>
         <rich>
-          <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-          <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+          <a:bodyPr/>
+          <a:p>
             <a:pPr>
               <a:defRPr/>
             </a:pPr>
@@ -1351,26 +1351,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$23</f>
+              <f>'Predictions'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$23</f>
+              <f>'Predictions'!$C$4:$C$24</f>
             </numRef>
           </val>
         </ser>
@@ -1383,26 +1383,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$23</f>
+              <f>'Predictions'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$H$4:$H$23</f>
+              <f>'Predictions'!$H$4:$H$24</f>
             </numRef>
           </val>
         </ser>
@@ -1415,26 +1415,26 @@
             </strRef>
           </tx>
           <spPr>
-            <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+            <a:ln>
               <a:prstDash val="solid"/>
             </a:ln>
           </spPr>
           <marker>
             <symbol val="none"/>
             <spPr>
-              <a:ln xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:ln>
                 <a:prstDash val="solid"/>
               </a:ln>
             </spPr>
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$23</f>
+              <f>'Predictions'!$B$4:$B$24</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$I$4:$I$23</f>
+              <f>'Predictions'!$I$4:$I$24</f>
             </numRef>
           </val>
         </ser>
@@ -1462,8 +1462,8 @@
         <title>
           <tx>
             <rich>
-              <a:bodyPr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main"/>
-              <a:p xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+              <a:bodyPr/>
+              <a:p>
                 <a:pPr>
                   <a:defRPr/>
                 </a:pPr>
@@ -1489,7 +1489,7 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>8</col>
@@ -1504,9 +1504,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1526,9 +1526,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1538,7 +1538,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>6</col>
@@ -1553,9 +1553,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1575,9 +1575,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1587,7 +1587,7 @@
 </file>
 
 <file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>7</col>
@@ -1602,9 +1602,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1614,7 +1614,7 @@
 </file>
 
 <file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>6</col>
@@ -1629,9 +1629,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1651,9 +1651,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1663,7 +1663,7 @@
 </file>
 
 <file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<wsDr xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+<wsDr xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <oneCellAnchor>
     <from>
       <col>9</col>
@@ -1678,9 +1678,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <c:chart r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -1700,9 +1700,9 @@
         <cNvGraphicFramePr/>
       </nvGraphicFramePr>
       <xfrm/>
-      <a:graphic xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+      <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+          <c:chart r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </graphicFrame>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>11:53:48 21/01/2026</t>
+          <t>14:32:42 21/01/2026</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$128.51</t>
+          <t>$127.21</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-2.43%</t>
+          <t>-1.30%</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$124.02</t>
+          <t>$122.57</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.044</t>
+          <t>0.013</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.54</t>
+          <t>0.57</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$127.52</t>
+          <t>$127.50</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>12.31%</t>
+          <t>12.19%</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>31.54</t>
+          <t>32.40</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.028</t>
+          <t>0.027</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN21"/>
+  <dimension ref="A1:AN22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5225,6 +5225,144 @@
         <v>0.54</v>
       </c>
     </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B22" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C22" t="n">
+        <v>127.21</v>
+      </c>
+      <c r="D22" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E22" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F22" t="n">
+        <v>-1.67</v>
+      </c>
+      <c r="G22" t="n">
+        <v>-1.296</v>
+      </c>
+      <c r="H22" t="n">
+        <v>2697859.957</v>
+      </c>
+      <c r="I22" t="n">
+        <v>344386807.26149</v>
+      </c>
+      <c r="J22" t="n">
+        <v>1356132</v>
+      </c>
+      <c r="K22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L22" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M22" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N22" t="n">
+        <v>7</v>
+      </c>
+      <c r="O22" t="n">
+        <v>2</v>
+      </c>
+      <c r="P22" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q22" t="n">
+        <v>1</v>
+      </c>
+      <c r="R22" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="S22" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T22" t="n">
+        <v>49.73</v>
+      </c>
+      <c r="U22" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V22" t="n">
+        <v>-0.8659</v>
+      </c>
+      <c r="W22" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X22" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="Y22" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Z22" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA22" t="n">
+        <v>58.2</v>
+      </c>
+      <c r="AB22" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC22" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="AD22" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="AE22" t="n">
+        <v>9.699999999999999</v>
+      </c>
+      <c r="AF22" t="n">
+        <v>122.57</v>
+      </c>
+      <c r="AG22" t="n">
+        <v>-3.65</v>
+      </c>
+      <c r="AH22" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI22" t="n">
+        <v>126.4</v>
+      </c>
+      <c r="AJ22" t="n">
+        <v>127.79</v>
+      </c>
+      <c r="AK22" t="n">
+        <v>126.4</v>
+      </c>
+      <c r="AL22" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM22" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN22" t="n">
+        <v>0.57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5236,7 +5374,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H23"/>
+  <dimension ref="A1:H24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5851,6 +5989,34 @@
       </c>
       <c r="H23" t="n">
         <v>3366014.115</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>127.21</v>
+      </c>
+      <c r="D24" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E24" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-1.67</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-1.296</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2697859.957</v>
       </c>
     </row>
   </sheetData>
@@ -5865,7 +6031,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6350,6 +6516,28 @@
       </c>
       <c r="F23" t="n">
         <v>-0.9674</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E24" t="n">
+        <v>49.73</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.8659</v>
       </c>
     </row>
   </sheetData>
@@ -6364,7 +6552,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:G24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6913,6 +7101,31 @@
         <v>7</v>
       </c>
       <c r="G23" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F24" t="n">
+        <v>7</v>
+      </c>
+      <c r="G24" t="n">
         <v>2</v>
       </c>
     </row>
@@ -6928,7 +7141,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7413,6 +7626,28 @@
       </c>
       <c r="F23" t="n">
         <v>57.9</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>0.013</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="E24" t="n">
+        <v>0</v>
+      </c>
+      <c r="F24" t="n">
+        <v>58.2</v>
       </c>
     </row>
   </sheetData>
@@ -7427,7 +7662,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I23"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8109,6 +8344,37 @@
         <v>129.4</v>
       </c>
     </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>14:32:42 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.60604952029</v>
+      </c>
+      <c r="C24" t="n">
+        <v>127.21</v>
+      </c>
+      <c r="D24" t="n">
+        <v>122.57</v>
+      </c>
+      <c r="E24" t="n">
+        <v>-3.65</v>
+      </c>
+      <c r="F24" t="n">
+        <v>0.451</v>
+      </c>
+      <c r="G24" t="n">
+        <v>0.549</v>
+      </c>
+      <c r="H24" t="n">
+        <v>126.4</v>
+      </c>
+      <c r="I24" t="n">
+        <v>127.79</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
ran a few more times
</commit_message>
<xml_diff>
--- a/tests/SOLUSDT_analysis.xlsx
+++ b/tests/SOLUSDT_analysis.xlsx
@@ -211,12 +211,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$24</f>
+              <f>'Price Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$C$4:$C$24</f>
+              <f>'Price Analysis'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -243,12 +243,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$24</f>
+              <f>'Price Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$D$4:$D$24</f>
+              <f>'Price Analysis'!$D$4:$D$29</f>
             </numRef>
           </val>
         </ser>
@@ -275,12 +275,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$24</f>
+              <f>'Price Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$E$4:$E$24</f>
+              <f>'Price Analysis'!$E$4:$E$29</f>
             </numRef>
           </val>
         </ser>
@@ -387,12 +387,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$24</f>
+              <f>'Price Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$H$4:$H$24</f>
+              <f>'Price Analysis'!$H$4:$H$29</f>
             </numRef>
           </val>
         </ser>
@@ -491,12 +491,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$24</f>
+              <f>'Technical Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$E$4:$E$24</f>
+              <f>'Technical Analysis'!$E$4:$E$29</f>
             </numRef>
           </val>
         </ser>
@@ -594,12 +594,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$24</f>
+              <f>'Technical Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$C$4:$C$24</f>
+              <f>'Technical Analysis'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -626,12 +626,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$24</f>
+              <f>'Technical Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$D$4:$D$24</f>
+              <f>'Technical Analysis'!$D$4:$D$29</f>
             </numRef>
           </val>
         </ser>
@@ -729,12 +729,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$24</f>
+              <f>'Fundamental Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$C$4:$C$24</f>
+              <f>'Fundamental Analysis'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -761,12 +761,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$24</f>
+              <f>'Fundamental Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$D$4:$D$24</f>
+              <f>'Fundamental Analysis'!$D$4:$D$29</f>
             </numRef>
           </val>
         </ser>
@@ -793,12 +793,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$24</f>
+              <f>'Fundamental Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$E$4:$E$24</f>
+              <f>'Fundamental Analysis'!$E$4:$E$29</f>
             </numRef>
           </val>
         </ser>
@@ -825,12 +825,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$24</f>
+              <f>'Fundamental Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$F$4:$F$24</f>
+              <f>'Fundamental Analysis'!$F$4:$F$29</f>
             </numRef>
           </val>
         </ser>
@@ -857,12 +857,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$24</f>
+              <f>'Fundamental Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$G$4:$G$24</f>
+              <f>'Fundamental Analysis'!$G$4:$G$29</f>
             </numRef>
           </val>
         </ser>
@@ -960,12 +960,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$24</f>
+              <f>'Sentiment Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$C$4:$C$24</f>
+              <f>'Sentiment Analysis'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -992,12 +992,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$24</f>
+              <f>'Sentiment Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$D$4:$D$24</f>
+              <f>'Sentiment Analysis'!$D$4:$D$29</f>
             </numRef>
           </val>
         </ser>
@@ -1024,12 +1024,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$24</f>
+              <f>'Sentiment Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$E$4:$E$24</f>
+              <f>'Sentiment Analysis'!$E$4:$E$29</f>
             </numRef>
           </val>
         </ser>
@@ -1127,12 +1127,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$24</f>
+              <f>'Sentiment Analysis'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$F$4:$F$24</f>
+              <f>'Sentiment Analysis'!$F$4:$F$29</f>
             </numRef>
           </val>
         </ser>
@@ -1230,12 +1230,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$24</f>
+              <f>'Predictions'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$24</f>
+              <f>'Predictions'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -1262,12 +1262,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$24</f>
+              <f>'Predictions'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$D$4:$D$24</f>
+              <f>'Predictions'!$D$4:$D$29</f>
             </numRef>
           </val>
         </ser>
@@ -1365,12 +1365,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$24</f>
+              <f>'Predictions'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$24</f>
+              <f>'Predictions'!$C$4:$C$29</f>
             </numRef>
           </val>
         </ser>
@@ -1397,12 +1397,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$24</f>
+              <f>'Predictions'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$H$4:$H$24</f>
+              <f>'Predictions'!$H$4:$H$29</f>
             </numRef>
           </val>
         </ser>
@@ -1429,12 +1429,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$24</f>
+              <f>'Predictions'!$B$4:$B$29</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$I$4:$I$24</f>
+              <f>'Predictions'!$I$4:$I$29</f>
             </numRef>
           </val>
         </ser>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>14:32:42 21/01/2026</t>
+          <t>22:41:11 21/01/2026</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$127.21</t>
+          <t>$126.44</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-1.30%</t>
+          <t>-0.77%</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$122.57</t>
+          <t>$122.41</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.013</t>
+          <t>-0.006</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.57</t>
+          <t>0.55</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>21</v>
+        <v>26</v>
       </c>
     </row>
     <row r="16">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$127.50</t>
+          <t>$127.68</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>12.19%</t>
+          <t>12.35%</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>32.40</t>
+          <t>37.31</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.027</t>
+          <t>0.022</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN22"/>
+  <dimension ref="A1:AN27"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5363,6 +5363,696 @@
         <v>0.57</v>
       </c>
     </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B23" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C23" t="n">
+        <v>127.56</v>
+      </c>
+      <c r="D23" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E23" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F23" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="G23" t="n">
+        <v>-1.391</v>
+      </c>
+      <c r="H23" t="n">
+        <v>2610341.411</v>
+      </c>
+      <c r="I23" t="n">
+        <v>332920971.88596</v>
+      </c>
+      <c r="J23" t="n">
+        <v>1307067</v>
+      </c>
+      <c r="K23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L23" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M23" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N23" t="n">
+        <v>7</v>
+      </c>
+      <c r="O23" t="n">
+        <v>2</v>
+      </c>
+      <c r="P23" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q23" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R23" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="S23" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T23" t="n">
+        <v>54.49</v>
+      </c>
+      <c r="U23" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V23" t="n">
+        <v>-0.7195</v>
+      </c>
+      <c r="W23" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X23" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="Y23" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="Z23" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA23" t="n">
+        <v>58.4</v>
+      </c>
+      <c r="AB23" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC23" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="AD23" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="AE23" t="n">
+        <v>9.109999999999999</v>
+      </c>
+      <c r="AF23" t="n">
+        <v>123.01</v>
+      </c>
+      <c r="AG23" t="n">
+        <v>-3.57</v>
+      </c>
+      <c r="AH23" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI23" t="n">
+        <v>127.37</v>
+      </c>
+      <c r="AJ23" t="n">
+        <v>128.24</v>
+      </c>
+      <c r="AK23" t="n">
+        <v>127.37</v>
+      </c>
+      <c r="AL23" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM23" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN23" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B24" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C24" t="n">
+        <v>129.05</v>
+      </c>
+      <c r="D24" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E24" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F24" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="G24" t="n">
+        <v>-0.023</v>
+      </c>
+      <c r="H24" t="n">
+        <v>2776039.268</v>
+      </c>
+      <c r="I24" t="n">
+        <v>353720271.19413</v>
+      </c>
+      <c r="J24" t="n">
+        <v>1376876</v>
+      </c>
+      <c r="K24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L24" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M24" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N24" t="n">
+        <v>7</v>
+      </c>
+      <c r="O24" t="n">
+        <v>2</v>
+      </c>
+      <c r="P24" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q24" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R24" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="S24" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T24" t="n">
+        <v>61.65</v>
+      </c>
+      <c r="U24" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V24" t="n">
+        <v>-0.5184</v>
+      </c>
+      <c r="W24" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X24" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="Y24" t="n">
+        <v>-0.008</v>
+      </c>
+      <c r="Z24" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA24" t="n">
+        <v>58.9</v>
+      </c>
+      <c r="AB24" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC24" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="AD24" t="n">
+        <v>0.526</v>
+      </c>
+      <c r="AE24" t="n">
+        <v>11.38</v>
+      </c>
+      <c r="AF24" t="n">
+        <v>124.75</v>
+      </c>
+      <c r="AG24" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="AH24" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI24" t="n">
+        <v>128.88</v>
+      </c>
+      <c r="AJ24" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="AK24" t="n">
+        <v>128.88</v>
+      </c>
+      <c r="AL24" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM24" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN24" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C25" t="n">
+        <v>129.09</v>
+      </c>
+      <c r="D25" t="n">
+        <v>129.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2775722.673</v>
+      </c>
+      <c r="I25" t="n">
+        <v>353672239.4001</v>
+      </c>
+      <c r="J25" t="n">
+        <v>1373155</v>
+      </c>
+      <c r="K25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L25" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N25" t="n">
+        <v>7</v>
+      </c>
+      <c r="O25" t="n">
+        <v>2</v>
+      </c>
+      <c r="P25" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q25" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R25" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="S25" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T25" t="n">
+        <v>61.85</v>
+      </c>
+      <c r="U25" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V25" t="n">
+        <v>-0.5152</v>
+      </c>
+      <c r="W25" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X25" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="Y25" t="n">
+        <v>-0.008</v>
+      </c>
+      <c r="Z25" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA25" t="n">
+        <v>58.9</v>
+      </c>
+      <c r="AB25" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC25" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="AD25" t="n">
+        <v>0.526</v>
+      </c>
+      <c r="AE25" t="n">
+        <v>11.46</v>
+      </c>
+      <c r="AF25" t="n">
+        <v>124.8</v>
+      </c>
+      <c r="AG25" t="n">
+        <v>-3.33</v>
+      </c>
+      <c r="AH25" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI25" t="n">
+        <v>128.89</v>
+      </c>
+      <c r="AJ25" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="AK25" t="n">
+        <v>128.89</v>
+      </c>
+      <c r="AL25" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM25" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN25" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C26" t="n">
+        <v>130.05</v>
+      </c>
+      <c r="D26" t="n">
+        <v>130.33</v>
+      </c>
+      <c r="E26" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F26" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2.112</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2732775.889</v>
+      </c>
+      <c r="I26" t="n">
+        <v>348314476.13076</v>
+      </c>
+      <c r="J26" t="n">
+        <v>1328020</v>
+      </c>
+      <c r="K26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L26" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N26" t="n">
+        <v>7</v>
+      </c>
+      <c r="O26" t="n">
+        <v>2</v>
+      </c>
+      <c r="P26" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="Q26" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R26" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="S26" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T26" t="n">
+        <v>65.95999999999999</v>
+      </c>
+      <c r="U26" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V26" t="n">
+        <v>-0.2616</v>
+      </c>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X26" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="Y26" t="n">
+        <v>-0.008999999999999999</v>
+      </c>
+      <c r="Z26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA26" t="n">
+        <v>60.5</v>
+      </c>
+      <c r="AB26" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC26" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="AD26" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="AE26" t="n">
+        <v>12.46</v>
+      </c>
+      <c r="AF26" t="n">
+        <v>126</v>
+      </c>
+      <c r="AG26" t="n">
+        <v>-3.11</v>
+      </c>
+      <c r="AH26" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI26" t="n">
+        <v>129.7</v>
+      </c>
+      <c r="AJ26" t="n">
+        <v>131.05</v>
+      </c>
+      <c r="AK26" t="n">
+        <v>129.7</v>
+      </c>
+      <c r="AL26" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM26" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN26" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C27" t="n">
+        <v>126.44</v>
+      </c>
+      <c r="D27" t="n">
+        <v>131.18</v>
+      </c>
+      <c r="E27" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.769</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2858599.373</v>
+      </c>
+      <c r="I27" t="n">
+        <v>365056668.42764</v>
+      </c>
+      <c r="J27" t="n">
+        <v>1359874</v>
+      </c>
+      <c r="K27" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L27" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M27" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N27" t="n">
+        <v>7</v>
+      </c>
+      <c r="O27" t="n">
+        <v>2</v>
+      </c>
+      <c r="P27" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q27" t="n">
+        <v>1</v>
+      </c>
+      <c r="R27" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="S27" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T27" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="U27" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V27" t="n">
+        <v>-0.4968</v>
+      </c>
+      <c r="W27" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X27" t="n">
+        <v>-0.006</v>
+      </c>
+      <c r="Y27" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="Z27" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA27" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="AB27" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC27" t="n">
+        <v>0.449</v>
+      </c>
+      <c r="AD27" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="AE27" t="n">
+        <v>20.65</v>
+      </c>
+      <c r="AF27" t="n">
+        <v>122.41</v>
+      </c>
+      <c r="AG27" t="n">
+        <v>-3.18</v>
+      </c>
+      <c r="AH27" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI27" t="n">
+        <v>125.16</v>
+      </c>
+      <c r="AJ27" t="n">
+        <v>127.64</v>
+      </c>
+      <c r="AK27" t="n">
+        <v>125.16</v>
+      </c>
+      <c r="AL27" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM27" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN27" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -5374,7 +6064,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H24"/>
+  <dimension ref="A1:H29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6017,6 +6707,146 @@
       </c>
       <c r="H24" t="n">
         <v>2697859.957</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C25" t="n">
+        <v>127.56</v>
+      </c>
+      <c r="D25" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E25" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-1.8</v>
+      </c>
+      <c r="G25" t="n">
+        <v>-1.391</v>
+      </c>
+      <c r="H25" t="n">
+        <v>2610341.411</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C26" t="n">
+        <v>129.05</v>
+      </c>
+      <c r="D26" t="n">
+        <v>129.77</v>
+      </c>
+      <c r="E26" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.03</v>
+      </c>
+      <c r="G26" t="n">
+        <v>-0.023</v>
+      </c>
+      <c r="H26" t="n">
+        <v>2776039.268</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C27" t="n">
+        <v>129.09</v>
+      </c>
+      <c r="D27" t="n">
+        <v>129.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="G27" t="n">
+        <v>-0.07000000000000001</v>
+      </c>
+      <c r="H27" t="n">
+        <v>2775722.673</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C28" t="n">
+        <v>130.05</v>
+      </c>
+      <c r="D28" t="n">
+        <v>130.33</v>
+      </c>
+      <c r="E28" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F28" t="n">
+        <v>2.69</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2.112</v>
+      </c>
+      <c r="H28" t="n">
+        <v>2732775.889</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C29" t="n">
+        <v>126.44</v>
+      </c>
+      <c r="D29" t="n">
+        <v>131.18</v>
+      </c>
+      <c r="E29" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.98</v>
+      </c>
+      <c r="G29" t="n">
+        <v>-0.769</v>
+      </c>
+      <c r="H29" t="n">
+        <v>2858599.373</v>
       </c>
     </row>
   </sheetData>
@@ -6031,7 +6861,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6538,6 +7368,116 @@
       </c>
       <c r="F24" t="n">
         <v>-0.8659</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E25" t="n">
+        <v>54.49</v>
+      </c>
+      <c r="F25" t="n">
+        <v>-0.7195</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C26" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.23</v>
+      </c>
+      <c r="E26" t="n">
+        <v>61.65</v>
+      </c>
+      <c r="F26" t="n">
+        <v>-0.5184</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C27" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D27" t="n">
+        <v>0.24</v>
+      </c>
+      <c r="E27" t="n">
+        <v>61.85</v>
+      </c>
+      <c r="F27" t="n">
+        <v>-0.5152</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D28" t="n">
+        <v>0.32</v>
+      </c>
+      <c r="E28" t="n">
+        <v>65.95999999999999</v>
+      </c>
+      <c r="F28" t="n">
+        <v>-0.2616</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C29" t="n">
+        <v>1</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.09</v>
+      </c>
+      <c r="E29" t="n">
+        <v>45.6</v>
+      </c>
+      <c r="F29" t="n">
+        <v>-0.4968</v>
       </c>
     </row>
   </sheetData>
@@ -6552,7 +7492,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G24"/>
+  <dimension ref="A1:G29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7126,6 +8066,131 @@
         <v>7</v>
       </c>
       <c r="G24" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F25" t="n">
+        <v>7</v>
+      </c>
+      <c r="G25" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E26" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>7</v>
+      </c>
+      <c r="G26" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C27" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D27" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E27" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F27" t="n">
+        <v>7</v>
+      </c>
+      <c r="G27" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D28" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F28" t="n">
+        <v>7</v>
+      </c>
+      <c r="G28" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D29" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F29" t="n">
+        <v>7</v>
+      </c>
+      <c r="G29" t="n">
         <v>2</v>
       </c>
     </row>
@@ -7141,7 +8206,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F24"/>
+  <dimension ref="A1:F29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7648,6 +8713,116 @@
       </c>
       <c r="F24" t="n">
         <v>58.2</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C25" t="n">
+        <v>0.024</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E25" t="n">
+        <v>0</v>
+      </c>
+      <c r="F25" t="n">
+        <v>58.4</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C26" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="D26" t="n">
+        <v>-0.008</v>
+      </c>
+      <c r="E26" t="n">
+        <v>0</v>
+      </c>
+      <c r="F26" t="n">
+        <v>58.9</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C27" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="D27" t="n">
+        <v>-0.008</v>
+      </c>
+      <c r="E27" t="n">
+        <v>0</v>
+      </c>
+      <c r="F27" t="n">
+        <v>58.9</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C28" t="n">
+        <v>-0.005</v>
+      </c>
+      <c r="D28" t="n">
+        <v>-0.008999999999999999</v>
+      </c>
+      <c r="E28" t="n">
+        <v>0</v>
+      </c>
+      <c r="F28" t="n">
+        <v>60.5</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C29" t="n">
+        <v>-0.006</v>
+      </c>
+      <c r="D29" t="n">
+        <v>-0.01</v>
+      </c>
+      <c r="E29" t="n">
+        <v>0</v>
+      </c>
+      <c r="F29" t="n">
+        <v>58.3</v>
       </c>
     </row>
   </sheetData>
@@ -7662,7 +8837,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I24"/>
+  <dimension ref="A1:I29"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8375,6 +9550,161 @@
         <v>127.79</v>
       </c>
     </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>16:40:09 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B25" s="5" t="n">
+        <v>46043.6945559778</v>
+      </c>
+      <c r="C25" t="n">
+        <v>127.56</v>
+      </c>
+      <c r="D25" t="n">
+        <v>123.01</v>
+      </c>
+      <c r="E25" t="n">
+        <v>-3.57</v>
+      </c>
+      <c r="F25" t="n">
+        <v>0.477</v>
+      </c>
+      <c r="G25" t="n">
+        <v>0.523</v>
+      </c>
+      <c r="H25" t="n">
+        <v>127.37</v>
+      </c>
+      <c r="I25" t="n">
+        <v>128.24</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>20:06:00 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B26" s="5" t="n">
+        <v>46043.83750339169</v>
+      </c>
+      <c r="C26" t="n">
+        <v>129.05</v>
+      </c>
+      <c r="D26" t="n">
+        <v>124.75</v>
+      </c>
+      <c r="E26" t="n">
+        <v>-3.34</v>
+      </c>
+      <c r="F26" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="G26" t="n">
+        <v>0.526</v>
+      </c>
+      <c r="H26" t="n">
+        <v>128.88</v>
+      </c>
+      <c r="I26" t="n">
+        <v>129.77</v>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>20:15:46 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B27" s="5" t="n">
+        <v>46043.8442848441</v>
+      </c>
+      <c r="C27" t="n">
+        <v>129.09</v>
+      </c>
+      <c r="D27" t="n">
+        <v>124.8</v>
+      </c>
+      <c r="E27" t="n">
+        <v>-3.33</v>
+      </c>
+      <c r="F27" t="n">
+        <v>0.474</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.526</v>
+      </c>
+      <c r="H27" t="n">
+        <v>128.89</v>
+      </c>
+      <c r="I27" t="n">
+        <v>129.77</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>20:40:43 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46043.86161179529</v>
+      </c>
+      <c r="C28" t="n">
+        <v>130.05</v>
+      </c>
+      <c r="D28" t="n">
+        <v>126</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-3.11</v>
+      </c>
+      <c r="F28" t="n">
+        <v>0.55</v>
+      </c>
+      <c r="G28" t="n">
+        <v>0.45</v>
+      </c>
+      <c r="H28" t="n">
+        <v>129.7</v>
+      </c>
+      <c r="I28" t="n">
+        <v>131.05</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>22:41:11 21/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46043.94527263061</v>
+      </c>
+      <c r="C29" t="n">
+        <v>126.44</v>
+      </c>
+      <c r="D29" t="n">
+        <v>122.41</v>
+      </c>
+      <c r="E29" t="n">
+        <v>-3.18</v>
+      </c>
+      <c r="F29" t="n">
+        <v>0.449</v>
+      </c>
+      <c r="G29" t="n">
+        <v>0.551</v>
+      </c>
+      <c r="H29" t="n">
+        <v>125.16</v>
+      </c>
+      <c r="I29" t="n">
+        <v>127.64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Added changes: working utility
</commit_message>
<xml_diff>
--- a/tests/SOLUSDT_analysis.xlsx
+++ b/tests/SOLUSDT_analysis.xlsx
@@ -211,12 +211,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$29</f>
+              <f>'Price Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$C$4:$C$29</f>
+              <f>'Price Analysis'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -243,12 +243,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$29</f>
+              <f>'Price Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$D$4:$D$29</f>
+              <f>'Price Analysis'!$D$4:$D$36</f>
             </numRef>
           </val>
         </ser>
@@ -275,12 +275,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$29</f>
+              <f>'Price Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$E$4:$E$29</f>
+              <f>'Price Analysis'!$E$4:$E$36</f>
             </numRef>
           </val>
         </ser>
@@ -387,12 +387,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$29</f>
+              <f>'Price Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$H$4:$H$29</f>
+              <f>'Price Analysis'!$H$4:$H$36</f>
             </numRef>
           </val>
         </ser>
@@ -491,12 +491,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$29</f>
+              <f>'Technical Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$E$4:$E$29</f>
+              <f>'Technical Analysis'!$E$4:$E$36</f>
             </numRef>
           </val>
         </ser>
@@ -594,12 +594,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$29</f>
+              <f>'Technical Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$C$4:$C$29</f>
+              <f>'Technical Analysis'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -626,12 +626,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$29</f>
+              <f>'Technical Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$D$4:$D$29</f>
+              <f>'Technical Analysis'!$D$4:$D$36</f>
             </numRef>
           </val>
         </ser>
@@ -729,12 +729,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$29</f>
+              <f>'Fundamental Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$C$4:$C$29</f>
+              <f>'Fundamental Analysis'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -761,12 +761,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$29</f>
+              <f>'Fundamental Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$D$4:$D$29</f>
+              <f>'Fundamental Analysis'!$D$4:$D$36</f>
             </numRef>
           </val>
         </ser>
@@ -793,12 +793,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$29</f>
+              <f>'Fundamental Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$E$4:$E$29</f>
+              <f>'Fundamental Analysis'!$E$4:$E$36</f>
             </numRef>
           </val>
         </ser>
@@ -825,12 +825,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$29</f>
+              <f>'Fundamental Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$F$4:$F$29</f>
+              <f>'Fundamental Analysis'!$F$4:$F$36</f>
             </numRef>
           </val>
         </ser>
@@ -857,12 +857,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$29</f>
+              <f>'Fundamental Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$G$4:$G$29</f>
+              <f>'Fundamental Analysis'!$G$4:$G$36</f>
             </numRef>
           </val>
         </ser>
@@ -960,12 +960,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$29</f>
+              <f>'Sentiment Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$C$4:$C$29</f>
+              <f>'Sentiment Analysis'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -992,12 +992,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$29</f>
+              <f>'Sentiment Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$D$4:$D$29</f>
+              <f>'Sentiment Analysis'!$D$4:$D$36</f>
             </numRef>
           </val>
         </ser>
@@ -1024,12 +1024,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$29</f>
+              <f>'Sentiment Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$E$4:$E$29</f>
+              <f>'Sentiment Analysis'!$E$4:$E$36</f>
             </numRef>
           </val>
         </ser>
@@ -1127,12 +1127,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$29</f>
+              <f>'Sentiment Analysis'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$F$4:$F$29</f>
+              <f>'Sentiment Analysis'!$F$4:$F$36</f>
             </numRef>
           </val>
         </ser>
@@ -1230,12 +1230,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$29</f>
+              <f>'Predictions'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$29</f>
+              <f>'Predictions'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -1262,12 +1262,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$29</f>
+              <f>'Predictions'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$D$4:$D$29</f>
+              <f>'Predictions'!$D$4:$D$36</f>
             </numRef>
           </val>
         </ser>
@@ -1365,12 +1365,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$29</f>
+              <f>'Predictions'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$29</f>
+              <f>'Predictions'!$C$4:$C$36</f>
             </numRef>
           </val>
         </ser>
@@ -1397,12 +1397,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$29</f>
+              <f>'Predictions'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$H$4:$H$29</f>
+              <f>'Predictions'!$H$4:$H$36</f>
             </numRef>
           </val>
         </ser>
@@ -1429,12 +1429,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$29</f>
+              <f>'Predictions'!$B$4:$B$36</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$I$4:$I$29</f>
+              <f>'Predictions'!$I$4:$I$36</f>
             </numRef>
           </val>
         </ser>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>22:41:11 21/01/2026</t>
+          <t>10:20:26 22/01/2026</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$126.44</t>
+          <t>$130.49</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>-0.77%</t>
+          <t>2.05%</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$122.41</t>
+          <t>$130.23</t>
         </is>
       </c>
     </row>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bearish</t>
+          <t>bullish</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>-0.006</t>
+          <t>0.049</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.55</t>
+          <t>0.62</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Hold or wait for clearer signals</t>
+          <t>Consider long position</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$127.68</t>
+          <t>$128.41</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>12.35%</t>
+          <t>14.84%</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>37.31</t>
+          <t>41.56</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.022</t>
+          <t>0.023</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN27"/>
+  <dimension ref="A1:AN34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6053,6 +6053,972 @@
         <v>0.55</v>
       </c>
     </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B28" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C28" t="n">
+        <v>131.34</v>
+      </c>
+      <c r="D28" t="n">
+        <v>131.45</v>
+      </c>
+      <c r="E28" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F28" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.417</v>
+      </c>
+      <c r="H28" t="n">
+        <v>3129151.403</v>
+      </c>
+      <c r="I28" t="n">
+        <v>400041652.26667</v>
+      </c>
+      <c r="J28" t="n">
+        <v>1522335</v>
+      </c>
+      <c r="K28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L28" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M28" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N28" t="n">
+        <v>7</v>
+      </c>
+      <c r="O28" t="n">
+        <v>2</v>
+      </c>
+      <c r="P28" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="Q28" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R28" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="S28" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T28" t="n">
+        <v>58.07</v>
+      </c>
+      <c r="U28" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V28" t="n">
+        <v>-0.1001</v>
+      </c>
+      <c r="W28" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X28" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y28" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA28" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="AB28" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC28" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="AD28" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="AE28" t="n">
+        <v>24.05</v>
+      </c>
+      <c r="AF28" t="n">
+        <v>127.91</v>
+      </c>
+      <c r="AG28" t="n">
+        <v>-2.61</v>
+      </c>
+      <c r="AH28" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI28" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="AJ28" t="n">
+        <v>132.28</v>
+      </c>
+      <c r="AK28" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="AL28" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM28" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN28" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B29" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C29" t="n">
+        <v>131.38</v>
+      </c>
+      <c r="D29" t="n">
+        <v>131.61</v>
+      </c>
+      <c r="E29" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F29" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="G29" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="H29" t="n">
+        <v>3163777.966</v>
+      </c>
+      <c r="I29" t="n">
+        <v>404605773.32788</v>
+      </c>
+      <c r="J29" t="n">
+        <v>1538906</v>
+      </c>
+      <c r="K29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L29" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M29" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N29" t="n">
+        <v>7</v>
+      </c>
+      <c r="O29" t="n">
+        <v>2</v>
+      </c>
+      <c r="P29" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="Q29" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R29" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="S29" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T29" t="n">
+        <v>58.14</v>
+      </c>
+      <c r="U29" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V29" t="n">
+        <v>-0.0977</v>
+      </c>
+      <c r="W29" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X29" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y29" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA29" t="n">
+        <v>62</v>
+      </c>
+      <c r="AB29" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC29" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="AD29" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="AE29" t="n">
+        <v>24.1</v>
+      </c>
+      <c r="AF29" t="n">
+        <v>127.94</v>
+      </c>
+      <c r="AG29" t="n">
+        <v>-2.61</v>
+      </c>
+      <c r="AH29" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI29" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="AJ29" t="n">
+        <v>132.28</v>
+      </c>
+      <c r="AK29" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="AL29" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM29" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN29" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C30" t="n">
+        <v>131.42</v>
+      </c>
+      <c r="D30" t="n">
+        <v>131.61</v>
+      </c>
+      <c r="E30" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3192315.455</v>
+      </c>
+      <c r="I30" t="n">
+        <v>408358699.34332</v>
+      </c>
+      <c r="J30" t="n">
+        <v>1551611</v>
+      </c>
+      <c r="K30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L30" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N30" t="n">
+        <v>7</v>
+      </c>
+      <c r="O30" t="n">
+        <v>2</v>
+      </c>
+      <c r="P30" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="Q30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="R30" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="S30" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T30" t="n">
+        <v>58.29</v>
+      </c>
+      <c r="U30" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V30" t="n">
+        <v>-0.0929</v>
+      </c>
+      <c r="W30" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X30" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y30" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA30" t="n">
+        <v>61.8</v>
+      </c>
+      <c r="AB30" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC30" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="AD30" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="AE30" t="n">
+        <v>24.21</v>
+      </c>
+      <c r="AF30" t="n">
+        <v>128</v>
+      </c>
+      <c r="AG30" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="AH30" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI30" t="n">
+        <v>130.23</v>
+      </c>
+      <c r="AJ30" t="n">
+        <v>132.28</v>
+      </c>
+      <c r="AK30" t="n">
+        <v>130.23</v>
+      </c>
+      <c r="AL30" t="n">
+        <v>0</v>
+      </c>
+      <c r="AM30" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN30" t="n">
+        <v>0.55</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C31" t="n">
+        <v>131.52</v>
+      </c>
+      <c r="D31" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E31" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3.502</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3205652.301</v>
+      </c>
+      <c r="I31" t="n">
+        <v>410129030.24927</v>
+      </c>
+      <c r="J31" t="n">
+        <v>1559785</v>
+      </c>
+      <c r="K31" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L31" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M31" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N31" t="n">
+        <v>7</v>
+      </c>
+      <c r="O31" t="n">
+        <v>2</v>
+      </c>
+      <c r="P31" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q31" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R31" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="S31" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T31" t="n">
+        <v>59.47</v>
+      </c>
+      <c r="U31" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V31" t="n">
+        <v>0.1819</v>
+      </c>
+      <c r="W31" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X31" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y31" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z31" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA31" t="n">
+        <v>62</v>
+      </c>
+      <c r="AB31" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC31" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="AD31" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="AE31" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="AF31" t="n">
+        <v>128.51</v>
+      </c>
+      <c r="AG31" t="n">
+        <v>-2.29</v>
+      </c>
+      <c r="AH31" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI31" t="n">
+        <v>131.15</v>
+      </c>
+      <c r="AJ31" t="n">
+        <v>132.67</v>
+      </c>
+      <c r="AK31" t="n">
+        <v>131.15</v>
+      </c>
+      <c r="AL31" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM31" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN31" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C32" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="D32" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E32" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F32" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3.141</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3232365.927</v>
+      </c>
+      <c r="I32" t="n">
+        <v>413648315.97641</v>
+      </c>
+      <c r="J32" t="n">
+        <v>1568143</v>
+      </c>
+      <c r="K32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L32" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N32" t="n">
+        <v>7</v>
+      </c>
+      <c r="O32" t="n">
+        <v>2</v>
+      </c>
+      <c r="P32" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q32" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R32" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="S32" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T32" t="n">
+        <v>57.79</v>
+      </c>
+      <c r="U32" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V32" t="n">
+        <v>0.1412</v>
+      </c>
+      <c r="W32" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X32" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y32" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z32" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA32" t="n">
+        <v>61.7</v>
+      </c>
+      <c r="AB32" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC32" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="AD32" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="AE32" t="n">
+        <v>24.07</v>
+      </c>
+      <c r="AF32" t="n">
+        <v>127.97</v>
+      </c>
+      <c r="AG32" t="n">
+        <v>-2.32</v>
+      </c>
+      <c r="AH32" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI32" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="AJ32" t="n">
+        <v>132.67</v>
+      </c>
+      <c r="AK32" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="AL32" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM32" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN32" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C33" t="n">
+        <v>130.61</v>
+      </c>
+      <c r="D33" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E33" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F33" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2.624</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3243674.964</v>
+      </c>
+      <c r="I33" t="n">
+        <v>415141055.79003</v>
+      </c>
+      <c r="J33" t="n">
+        <v>1576177</v>
+      </c>
+      <c r="K33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L33" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N33" t="n">
+        <v>7</v>
+      </c>
+      <c r="O33" t="n">
+        <v>2</v>
+      </c>
+      <c r="P33" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q33" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R33" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="S33" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T33" t="n">
+        <v>56.51</v>
+      </c>
+      <c r="U33" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V33" t="n">
+        <v>0.1093</v>
+      </c>
+      <c r="W33" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X33" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="Y33" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="Z33" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA33" t="n">
+        <v>61.3</v>
+      </c>
+      <c r="AB33" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC33" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="AD33" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="AE33" t="n">
+        <v>24.23</v>
+      </c>
+      <c r="AF33" t="n">
+        <v>127.55</v>
+      </c>
+      <c r="AG33" t="n">
+        <v>-2.34</v>
+      </c>
+      <c r="AH33" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI33" t="n">
+        <v>129.57</v>
+      </c>
+      <c r="AJ33" t="n">
+        <v>130.91</v>
+      </c>
+      <c r="AK33" t="n">
+        <v>129.57</v>
+      </c>
+      <c r="AL33" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM33" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN33" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C34" t="n">
+        <v>130.49</v>
+      </c>
+      <c r="D34" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E34" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F34" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2.049</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3076104.036</v>
+      </c>
+      <c r="I34" t="n">
+        <v>396518874.96492</v>
+      </c>
+      <c r="J34" t="n">
+        <v>1542990</v>
+      </c>
+      <c r="K34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L34" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N34" t="n">
+        <v>7</v>
+      </c>
+      <c r="O34" t="n">
+        <v>2</v>
+      </c>
+      <c r="P34" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q34" t="n">
+        <v>1</v>
+      </c>
+      <c r="R34" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="S34" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="T34" t="n">
+        <v>53.04</v>
+      </c>
+      <c r="U34" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V34" t="n">
+        <v>0.4808</v>
+      </c>
+      <c r="W34" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X34" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="Y34" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="Z34" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA34" t="n">
+        <v>52.4</v>
+      </c>
+      <c r="AB34" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC34" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="AD34" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="AE34" t="n">
+        <v>24.13</v>
+      </c>
+      <c r="AF34" t="n">
+        <v>130.23</v>
+      </c>
+      <c r="AG34" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="AH34" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI34" t="n">
+        <v>129.24</v>
+      </c>
+      <c r="AJ34" t="n">
+        <v>130.65</v>
+      </c>
+      <c r="AK34" t="n">
+        <v>129.24</v>
+      </c>
+      <c r="AL34" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM34" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN34" t="n">
+        <v>0.62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -6064,7 +7030,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H29"/>
+  <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -6847,6 +7813,202 @@
       </c>
       <c r="H29" t="n">
         <v>2858599.373</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C30" t="n">
+        <v>131.34</v>
+      </c>
+      <c r="D30" t="n">
+        <v>131.45</v>
+      </c>
+      <c r="E30" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F30" t="n">
+        <v>4.34</v>
+      </c>
+      <c r="G30" t="n">
+        <v>3.417</v>
+      </c>
+      <c r="H30" t="n">
+        <v>3129151.403</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C31" t="n">
+        <v>131.38</v>
+      </c>
+      <c r="D31" t="n">
+        <v>131.61</v>
+      </c>
+      <c r="E31" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F31" t="n">
+        <v>4.43</v>
+      </c>
+      <c r="G31" t="n">
+        <v>3.49</v>
+      </c>
+      <c r="H31" t="n">
+        <v>3163777.966</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C32" t="n">
+        <v>131.42</v>
+      </c>
+      <c r="D32" t="n">
+        <v>131.61</v>
+      </c>
+      <c r="E32" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F32" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="G32" t="n">
+        <v>3.22</v>
+      </c>
+      <c r="H32" t="n">
+        <v>3192315.455</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C33" t="n">
+        <v>131.52</v>
+      </c>
+      <c r="D33" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E33" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F33" t="n">
+        <v>4.45</v>
+      </c>
+      <c r="G33" t="n">
+        <v>3.502</v>
+      </c>
+      <c r="H33" t="n">
+        <v>3205652.301</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C34" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="D34" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E34" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F34" t="n">
+        <v>3.99</v>
+      </c>
+      <c r="G34" t="n">
+        <v>3.141</v>
+      </c>
+      <c r="H34" t="n">
+        <v>3232365.927</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C35" t="n">
+        <v>130.61</v>
+      </c>
+      <c r="D35" t="n">
+        <v>131.68</v>
+      </c>
+      <c r="E35" t="n">
+        <v>124.68</v>
+      </c>
+      <c r="F35" t="n">
+        <v>3.34</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2.624</v>
+      </c>
+      <c r="H35" t="n">
+        <v>3243674.964</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C36" t="n">
+        <v>130.49</v>
+      </c>
+      <c r="D36" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E36" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F36" t="n">
+        <v>2.62</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2.049</v>
+      </c>
+      <c r="H36" t="n">
+        <v>3076104.036</v>
       </c>
     </row>
   </sheetData>
@@ -6861,7 +8023,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7478,6 +8640,160 @@
       </c>
       <c r="F29" t="n">
         <v>-0.4968</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E30" t="n">
+        <v>58.07</v>
+      </c>
+      <c r="F30" t="n">
+        <v>-0.1001</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E31" t="n">
+        <v>58.14</v>
+      </c>
+      <c r="F31" t="n">
+        <v>-0.0977</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="E32" t="n">
+        <v>58.29</v>
+      </c>
+      <c r="F32" t="n">
+        <v>-0.0929</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.19</v>
+      </c>
+      <c r="E33" t="n">
+        <v>59.47</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.1819</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="E34" t="n">
+        <v>57.79</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.1412</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.13</v>
+      </c>
+      <c r="E35" t="n">
+        <v>56.51</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.1093</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C36" t="n">
+        <v>1</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="E36" t="n">
+        <v>53.04</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.4808</v>
       </c>
     </row>
   </sheetData>
@@ -7492,7 +8808,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G29"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8191,6 +9507,181 @@
         <v>7</v>
       </c>
       <c r="G29" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E30" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F30" t="n">
+        <v>7</v>
+      </c>
+      <c r="G30" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C31" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E31" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F31" t="n">
+        <v>7</v>
+      </c>
+      <c r="G31" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E32" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F32" t="n">
+        <v>7</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D33" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E33" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F33" t="n">
+        <v>7</v>
+      </c>
+      <c r="G33" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D34" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E34" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F34" t="n">
+        <v>7</v>
+      </c>
+      <c r="G34" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C35" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D35" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E35" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F35" t="n">
+        <v>7</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D36" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F36" t="n">
+        <v>7</v>
+      </c>
+      <c r="G36" t="n">
         <v>2</v>
       </c>
     </row>
@@ -8206,7 +9697,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F29"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8823,6 +10314,160 @@
       </c>
       <c r="F29" t="n">
         <v>58.3</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C30" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D30" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E30" t="n">
+        <v>0</v>
+      </c>
+      <c r="F30" t="n">
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C31" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D31" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E31" t="n">
+        <v>0</v>
+      </c>
+      <c r="F31" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C32" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D32" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E32" t="n">
+        <v>0</v>
+      </c>
+      <c r="F32" t="n">
+        <v>61.8</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C33" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D33" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E33" t="n">
+        <v>0</v>
+      </c>
+      <c r="F33" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C34" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D34" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E34" t="n">
+        <v>0</v>
+      </c>
+      <c r="F34" t="n">
+        <v>61.7</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C35" t="n">
+        <v>0.022</v>
+      </c>
+      <c r="D35" t="n">
+        <v>0.036</v>
+      </c>
+      <c r="E35" t="n">
+        <v>0</v>
+      </c>
+      <c r="F35" t="n">
+        <v>61.3</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C36" t="n">
+        <v>0.049</v>
+      </c>
+      <c r="D36" t="n">
+        <v>0.082</v>
+      </c>
+      <c r="E36" t="n">
+        <v>0</v>
+      </c>
+      <c r="F36" t="n">
+        <v>52.4</v>
       </c>
     </row>
   </sheetData>
@@ -8837,7 +10482,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9705,6 +11350,223 @@
         <v>127.64</v>
       </c>
     </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>01:15:29 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B30" s="5" t="n">
+        <v>46044.05241941915</v>
+      </c>
+      <c r="C30" t="n">
+        <v>131.34</v>
+      </c>
+      <c r="D30" t="n">
+        <v>127.91</v>
+      </c>
+      <c r="E30" t="n">
+        <v>-2.61</v>
+      </c>
+      <c r="F30" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="G30" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="H30" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="I30" t="n">
+        <v>132.28</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>01:20:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B31" s="5" t="n">
+        <v>46044.05588241426</v>
+      </c>
+      <c r="C31" t="n">
+        <v>131.38</v>
+      </c>
+      <c r="D31" t="n">
+        <v>127.94</v>
+      </c>
+      <c r="E31" t="n">
+        <v>-2.61</v>
+      </c>
+      <c r="F31" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="G31" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="H31" t="n">
+        <v>130.22</v>
+      </c>
+      <c r="I31" t="n">
+        <v>132.28</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>01:25:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B32" s="5" t="n">
+        <v>46044.0593591213</v>
+      </c>
+      <c r="C32" t="n">
+        <v>131.42</v>
+      </c>
+      <c r="D32" t="n">
+        <v>128</v>
+      </c>
+      <c r="E32" t="n">
+        <v>-2.6</v>
+      </c>
+      <c r="F32" t="n">
+        <v>0.552</v>
+      </c>
+      <c r="G32" t="n">
+        <v>0.448</v>
+      </c>
+      <c r="H32" t="n">
+        <v>130.23</v>
+      </c>
+      <c r="I32" t="n">
+        <v>132.28</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>01:30:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B33" s="5" t="n">
+        <v>46044.06283290812</v>
+      </c>
+      <c r="C33" t="n">
+        <v>131.52</v>
+      </c>
+      <c r="D33" t="n">
+        <v>128.51</v>
+      </c>
+      <c r="E33" t="n">
+        <v>-2.29</v>
+      </c>
+      <c r="F33" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="G33" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="H33" t="n">
+        <v>131.15</v>
+      </c>
+      <c r="I33" t="n">
+        <v>132.67</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>01:35:28 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B34" s="5" t="n">
+        <v>46044.06629963835</v>
+      </c>
+      <c r="C34" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="D34" t="n">
+        <v>127.97</v>
+      </c>
+      <c r="E34" t="n">
+        <v>-2.32</v>
+      </c>
+      <c r="F34" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="G34" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="H34" t="n">
+        <v>131.01</v>
+      </c>
+      <c r="I34" t="n">
+        <v>132.67</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>01:40:27 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.06976695727</v>
+      </c>
+      <c r="C35" t="n">
+        <v>130.61</v>
+      </c>
+      <c r="D35" t="n">
+        <v>127.55</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-2.34</v>
+      </c>
+      <c r="F35" t="n">
+        <v>0.627</v>
+      </c>
+      <c r="G35" t="n">
+        <v>0.373</v>
+      </c>
+      <c r="H35" t="n">
+        <v>129.57</v>
+      </c>
+      <c r="I35" t="n">
+        <v>130.91</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>10:20:26 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.4308623914</v>
+      </c>
+      <c r="C36" t="n">
+        <v>130.49</v>
+      </c>
+      <c r="D36" t="n">
+        <v>130.23</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="F36" t="n">
+        <v>0.655</v>
+      </c>
+      <c r="G36" t="n">
+        <v>0.345</v>
+      </c>
+      <c r="H36" t="n">
+        <v>129.24</v>
+      </c>
+      <c r="I36" t="n">
+        <v>130.65</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>

<commit_message>
Few more executions for SOLUSDT
</commit_message>
<xml_diff>
--- a/tests/SOLUSDT_analysis.xlsx
+++ b/tests/SOLUSDT_analysis.xlsx
@@ -211,12 +211,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$36</f>
+              <f>'Price Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$C$4:$C$36</f>
+              <f>'Price Analysis'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -243,12 +243,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$36</f>
+              <f>'Price Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$D$4:$D$36</f>
+              <f>'Price Analysis'!$D$4:$D$45</f>
             </numRef>
           </val>
         </ser>
@@ -275,12 +275,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$36</f>
+              <f>'Price Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$E$4:$E$36</f>
+              <f>'Price Analysis'!$E$4:$E$45</f>
             </numRef>
           </val>
         </ser>
@@ -387,12 +387,12 @@
           </spPr>
           <cat>
             <numRef>
-              <f>'Price Analysis'!$B$4:$B$36</f>
+              <f>'Price Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Price Analysis'!$H$4:$H$36</f>
+              <f>'Price Analysis'!$H$4:$H$45</f>
             </numRef>
           </val>
         </ser>
@@ -491,12 +491,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$36</f>
+              <f>'Technical Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$E$4:$E$36</f>
+              <f>'Technical Analysis'!$E$4:$E$45</f>
             </numRef>
           </val>
         </ser>
@@ -594,12 +594,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$36</f>
+              <f>'Technical Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$C$4:$C$36</f>
+              <f>'Technical Analysis'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -626,12 +626,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Technical Analysis'!$B$4:$B$36</f>
+              <f>'Technical Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Technical Analysis'!$D$4:$D$36</f>
+              <f>'Technical Analysis'!$D$4:$D$45</f>
             </numRef>
           </val>
         </ser>
@@ -729,12 +729,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$36</f>
+              <f>'Fundamental Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$C$4:$C$36</f>
+              <f>'Fundamental Analysis'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -761,12 +761,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$36</f>
+              <f>'Fundamental Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$D$4:$D$36</f>
+              <f>'Fundamental Analysis'!$D$4:$D$45</f>
             </numRef>
           </val>
         </ser>
@@ -793,12 +793,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$36</f>
+              <f>'Fundamental Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$E$4:$E$36</f>
+              <f>'Fundamental Analysis'!$E$4:$E$45</f>
             </numRef>
           </val>
         </ser>
@@ -825,12 +825,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$36</f>
+              <f>'Fundamental Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$F$4:$F$36</f>
+              <f>'Fundamental Analysis'!$F$4:$F$45</f>
             </numRef>
           </val>
         </ser>
@@ -857,12 +857,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Fundamental Analysis'!$B$4:$B$36</f>
+              <f>'Fundamental Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Fundamental Analysis'!$G$4:$G$36</f>
+              <f>'Fundamental Analysis'!$G$4:$G$45</f>
             </numRef>
           </val>
         </ser>
@@ -960,12 +960,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$36</f>
+              <f>'Sentiment Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$C$4:$C$36</f>
+              <f>'Sentiment Analysis'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -992,12 +992,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$36</f>
+              <f>'Sentiment Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$D$4:$D$36</f>
+              <f>'Sentiment Analysis'!$D$4:$D$45</f>
             </numRef>
           </val>
         </ser>
@@ -1024,12 +1024,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$36</f>
+              <f>'Sentiment Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$E$4:$E$36</f>
+              <f>'Sentiment Analysis'!$E$4:$E$45</f>
             </numRef>
           </val>
         </ser>
@@ -1127,12 +1127,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Sentiment Analysis'!$B$4:$B$36</f>
+              <f>'Sentiment Analysis'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Sentiment Analysis'!$F$4:$F$36</f>
+              <f>'Sentiment Analysis'!$F$4:$F$45</f>
             </numRef>
           </val>
         </ser>
@@ -1230,12 +1230,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$36</f>
+              <f>'Predictions'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$36</f>
+              <f>'Predictions'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -1262,12 +1262,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$36</f>
+              <f>'Predictions'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$D$4:$D$36</f>
+              <f>'Predictions'!$D$4:$D$45</f>
             </numRef>
           </val>
         </ser>
@@ -1365,12 +1365,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$36</f>
+              <f>'Predictions'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$C$4:$C$36</f>
+              <f>'Predictions'!$C$4:$C$45</f>
             </numRef>
           </val>
         </ser>
@@ -1397,12 +1397,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$36</f>
+              <f>'Predictions'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$H$4:$H$36</f>
+              <f>'Predictions'!$H$4:$H$45</f>
             </numRef>
           </val>
         </ser>
@@ -1429,12 +1429,12 @@
           </marker>
           <cat>
             <numRef>
-              <f>'Predictions'!$B$4:$B$36</f>
+              <f>'Predictions'!$B$4:$B$45</f>
             </numRef>
           </cat>
           <val>
             <numRef>
-              <f>'Predictions'!$I$4:$I$36</f>
+              <f>'Predictions'!$I$4:$I$45</f>
             </numRef>
           </val>
         </ser>
@@ -2034,7 +2034,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>10:20:26 22/01/2026</t>
+          <t>07:58:29 29/01/2026</t>
         </is>
       </c>
     </row>
@@ -2046,7 +2046,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>$130.49</t>
+          <t>$124.50</t>
         </is>
       </c>
     </row>
@@ -2058,7 +2058,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>2.05%</t>
+          <t>-2.14%</t>
         </is>
       </c>
     </row>
@@ -2070,7 +2070,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>$130.23</t>
+          <t>$125.52</t>
         </is>
       </c>
     </row>
@@ -2082,7 +2082,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>bullish</t>
+          <t>bearish</t>
         </is>
       </c>
     </row>
@@ -2094,7 +2094,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>0.049</t>
+          <t>0.108</t>
         </is>
       </c>
     </row>
@@ -2106,7 +2106,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>0.62</t>
+          <t>0.53</t>
         </is>
       </c>
     </row>
@@ -2118,7 +2118,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Consider long position</t>
+          <t>Hold or wait for clearer signals</t>
         </is>
       </c>
     </row>
@@ -2136,7 +2136,7 @@
         </is>
       </c>
       <c r="B15" t="n">
-        <v>33</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
@@ -2147,7 +2147,7 @@
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>$128.41</t>
+          <t>$128.02</t>
         </is>
       </c>
     </row>
@@ -2171,7 +2171,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>14.84%</t>
+          <t>14.08%</t>
         </is>
       </c>
     </row>
@@ -2183,7 +2183,7 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>41.56</t>
+          <t>40.54</t>
         </is>
       </c>
     </row>
@@ -2195,7 +2195,7 @@
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>0.023</t>
+          <t>0.029</t>
         </is>
       </c>
     </row>
@@ -2213,7 +2213,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AN34"/>
+  <dimension ref="A1:AN43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7019,6 +7019,1248 @@
         <v>0.62</v>
       </c>
     </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B35" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C35" t="n">
+        <v>130.15</v>
+      </c>
+      <c r="D35" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E35" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F35" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G35" t="n">
+        <v>2.038</v>
+      </c>
+      <c r="H35" t="n">
+        <v>2949879.654</v>
+      </c>
+      <c r="I35" t="n">
+        <v>380824894.96739</v>
+      </c>
+      <c r="J35" t="n">
+        <v>1514253</v>
+      </c>
+      <c r="K35" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L35" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M35" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N35" t="n">
+        <v>7</v>
+      </c>
+      <c r="O35" t="n">
+        <v>2</v>
+      </c>
+      <c r="P35" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q35" t="n">
+        <v>1</v>
+      </c>
+      <c r="R35" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="S35" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T35" t="n">
+        <v>36.63</v>
+      </c>
+      <c r="U35" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V35" t="n">
+        <v>0.3967</v>
+      </c>
+      <c r="W35" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X35" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="Y35" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="Z35" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA35" t="n">
+        <v>61.9</v>
+      </c>
+      <c r="AB35" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC35" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="AD35" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="AE35" t="n">
+        <v>23.96</v>
+      </c>
+      <c r="AF35" t="n">
+        <v>131.44</v>
+      </c>
+      <c r="AG35" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="AH35" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI35" t="n">
+        <v>129.96</v>
+      </c>
+      <c r="AJ35" t="n">
+        <v>130.59</v>
+      </c>
+      <c r="AK35" t="n">
+        <v>129.96</v>
+      </c>
+      <c r="AL35" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM35" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN35" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B36" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C36" t="n">
+        <v>130.17</v>
+      </c>
+      <c r="D36" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E36" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F36" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="G36" t="n">
+        <v>2.609</v>
+      </c>
+      <c r="H36" t="n">
+        <v>2904901.346</v>
+      </c>
+      <c r="I36" t="n">
+        <v>375342537.63177</v>
+      </c>
+      <c r="J36" t="n">
+        <v>1502808</v>
+      </c>
+      <c r="K36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L36" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M36" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N36" t="n">
+        <v>7</v>
+      </c>
+      <c r="O36" t="n">
+        <v>2</v>
+      </c>
+      <c r="P36" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q36" t="n">
+        <v>1</v>
+      </c>
+      <c r="R36" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="S36" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T36" t="n">
+        <v>44.73</v>
+      </c>
+      <c r="U36" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V36" t="n">
+        <v>0.3562</v>
+      </c>
+      <c r="W36" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="X36" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="Y36" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="Z36" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA36" t="n">
+        <v>62.3</v>
+      </c>
+      <c r="AB36" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC36" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="AD36" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="AE36" t="n">
+        <v>14.92</v>
+      </c>
+      <c r="AF36" t="n">
+        <v>131.81</v>
+      </c>
+      <c r="AG36" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="AH36" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI36" t="n">
+        <v>129.83</v>
+      </c>
+      <c r="AJ36" t="n">
+        <v>130.69</v>
+      </c>
+      <c r="AK36" t="n">
+        <v>129.83</v>
+      </c>
+      <c r="AL36" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM36" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN36" t="n">
+        <v>0.57</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C37" t="n">
+        <v>128.12</v>
+      </c>
+      <c r="D37" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E37" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F37" t="n">
+        <v>-2.57</v>
+      </c>
+      <c r="G37" t="n">
+        <v>-1.966</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2634025.992</v>
+      </c>
+      <c r="I37" t="n">
+        <v>340813711.23301</v>
+      </c>
+      <c r="J37" t="n">
+        <v>1408508</v>
+      </c>
+      <c r="K37" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L37" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M37" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N37" t="n">
+        <v>7</v>
+      </c>
+      <c r="O37" t="n">
+        <v>2</v>
+      </c>
+      <c r="P37" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q37" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R37" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S37" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T37" t="n">
+        <v>28.04</v>
+      </c>
+      <c r="U37" t="inlineStr">
+        <is>
+          <t>oversold</t>
+        </is>
+      </c>
+      <c r="V37" t="n">
+        <v>-0.0298</v>
+      </c>
+      <c r="W37" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="X37" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="Y37" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="Z37" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA37" t="n">
+        <v>58.3</v>
+      </c>
+      <c r="AB37" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC37" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="AD37" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="AE37" t="n">
+        <v>7.41</v>
+      </c>
+      <c r="AF37" t="n">
+        <v>129.8</v>
+      </c>
+      <c r="AG37" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="AH37" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI37" t="n">
+        <v>127.33</v>
+      </c>
+      <c r="AJ37" t="n">
+        <v>128.96</v>
+      </c>
+      <c r="AK37" t="n">
+        <v>127.33</v>
+      </c>
+      <c r="AL37" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM37" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN37" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C38" t="n">
+        <v>127.93</v>
+      </c>
+      <c r="D38" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E38" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2537841.581</v>
+      </c>
+      <c r="I38" t="n">
+        <v>327798379.49668</v>
+      </c>
+      <c r="J38" t="n">
+        <v>1393732</v>
+      </c>
+      <c r="K38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L38" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N38" t="n">
+        <v>7</v>
+      </c>
+      <c r="O38" t="n">
+        <v>2</v>
+      </c>
+      <c r="P38" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q38" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R38" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="S38" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T38" t="n">
+        <v>32.05</v>
+      </c>
+      <c r="U38" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V38" t="n">
+        <v>-0.1863</v>
+      </c>
+      <c r="W38" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="X38" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="Y38" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="Z38" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA38" t="n">
+        <v>60.2</v>
+      </c>
+      <c r="AB38" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC38" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="AD38" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="AE38" t="n">
+        <v>7.73</v>
+      </c>
+      <c r="AF38" t="n">
+        <v>129.55</v>
+      </c>
+      <c r="AG38" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="AH38" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI38" t="n">
+        <v>127.87</v>
+      </c>
+      <c r="AJ38" t="n">
+        <v>128.97</v>
+      </c>
+      <c r="AK38" t="n">
+        <v>127.87</v>
+      </c>
+      <c r="AL38" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM38" t="inlineStr">
+        <is>
+          <t>Consider short position or avoid</t>
+        </is>
+      </c>
+      <c r="AN38" t="n">
+        <v>0.58</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C39" t="n">
+        <v>128.17</v>
+      </c>
+      <c r="D39" t="n">
+        <v>129.76</v>
+      </c>
+      <c r="E39" t="n">
+        <v>125.28</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="H39" t="n">
+        <v>1904825.519</v>
+      </c>
+      <c r="I39" t="n">
+        <v>243476909.56405</v>
+      </c>
+      <c r="J39" t="n">
+        <v>944550</v>
+      </c>
+      <c r="K39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L39" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N39" t="n">
+        <v>7</v>
+      </c>
+      <c r="O39" t="n">
+        <v>2</v>
+      </c>
+      <c r="P39" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q39" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R39" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="S39" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T39" t="n">
+        <v>46.15</v>
+      </c>
+      <c r="U39" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V39" t="n">
+        <v>-0.3144</v>
+      </c>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X39" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="Y39" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="Z39" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA39" t="n">
+        <v>57.1</v>
+      </c>
+      <c r="AB39" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC39" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="AD39" t="n">
+        <v>0.537</v>
+      </c>
+      <c r="AE39" t="n">
+        <v>9.98</v>
+      </c>
+      <c r="AF39" t="n">
+        <v>126.92</v>
+      </c>
+      <c r="AG39" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="AH39" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI39" t="n">
+        <v>127.71</v>
+      </c>
+      <c r="AJ39" t="n">
+        <v>129.24</v>
+      </c>
+      <c r="AK39" t="n">
+        <v>127.71</v>
+      </c>
+      <c r="AL39" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM39" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN39" t="n">
+        <v>0.54</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C40" t="n">
+        <v>120.91</v>
+      </c>
+      <c r="D40" t="n">
+        <v>127.76</v>
+      </c>
+      <c r="E40" t="n">
+        <v>120.44</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-6.38</v>
+      </c>
+      <c r="G40" t="n">
+        <v>-5.012</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2248082.51</v>
+      </c>
+      <c r="I40" t="n">
+        <v>278927928.35689</v>
+      </c>
+      <c r="J40" t="n">
+        <v>771751</v>
+      </c>
+      <c r="K40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L40" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N40" t="n">
+        <v>7</v>
+      </c>
+      <c r="O40" t="n">
+        <v>2</v>
+      </c>
+      <c r="P40" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q40" t="n">
+        <v>1</v>
+      </c>
+      <c r="R40" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S40" t="inlineStr">
+        <is>
+          <t>medium</t>
+        </is>
+      </c>
+      <c r="T40" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="U40" t="inlineStr">
+        <is>
+          <t>oversold</t>
+        </is>
+      </c>
+      <c r="V40" t="n">
+        <v>-1.2877</v>
+      </c>
+      <c r="W40" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="X40" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="Y40" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="Z40" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA40" t="n">
+        <v>47.9</v>
+      </c>
+      <c r="AB40" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC40" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="AD40" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="AE40" t="n">
+        <v>10.45</v>
+      </c>
+      <c r="AF40" t="n">
+        <v>119.22</v>
+      </c>
+      <c r="AG40" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="AH40" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI40" t="n">
+        <v>120.85</v>
+      </c>
+      <c r="AJ40" t="n">
+        <v>122.04</v>
+      </c>
+      <c r="AK40" t="n">
+        <v>120.85</v>
+      </c>
+      <c r="AL40" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM40" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN40" t="n">
+        <v>0.5600000000000001</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C41" t="n">
+        <v>124.19</v>
+      </c>
+      <c r="D41" t="n">
+        <v>125.6</v>
+      </c>
+      <c r="E41" t="n">
+        <v>121.76</v>
+      </c>
+      <c r="F41" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="G41" t="n">
+        <v>1.264</v>
+      </c>
+      <c r="H41" t="n">
+        <v>2052108.573</v>
+      </c>
+      <c r="I41" t="n">
+        <v>253911779.72656</v>
+      </c>
+      <c r="J41" t="n">
+        <v>1013823</v>
+      </c>
+      <c r="K41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L41" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N41" t="n">
+        <v>7</v>
+      </c>
+      <c r="O41" t="n">
+        <v>2</v>
+      </c>
+      <c r="P41" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q41" t="n">
+        <v>1</v>
+      </c>
+      <c r="R41" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="S41" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T41" t="n">
+        <v>55.79</v>
+      </c>
+      <c r="U41" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V41" t="n">
+        <v>0.3556</v>
+      </c>
+      <c r="W41" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X41" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="Y41" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="Z41" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA41" t="n">
+        <v>62</v>
+      </c>
+      <c r="AB41" t="inlineStr">
+        <is>
+          <t>Greed</t>
+        </is>
+      </c>
+      <c r="AC41" t="n">
+        <v>0.662</v>
+      </c>
+      <c r="AD41" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="AE41" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="AF41" t="n">
+        <v>123.59</v>
+      </c>
+      <c r="AG41" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="AH41" t="inlineStr">
+        <is>
+          <t>downward</t>
+        </is>
+      </c>
+      <c r="AI41" t="n">
+        <v>123.84</v>
+      </c>
+      <c r="AJ41" t="n">
+        <v>124.97</v>
+      </c>
+      <c r="AK41" t="n">
+        <v>123.84</v>
+      </c>
+      <c r="AL41" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM41" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN41" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C42" t="n">
+        <v>125.15</v>
+      </c>
+      <c r="D42" t="n">
+        <v>126.79</v>
+      </c>
+      <c r="E42" t="n">
+        <v>123.12</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="H42" t="n">
+        <v>1788683.963</v>
+      </c>
+      <c r="I42" t="n">
+        <v>222754300.31417</v>
+      </c>
+      <c r="J42" t="n">
+        <v>939410</v>
+      </c>
+      <c r="K42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L42" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N42" t="n">
+        <v>7</v>
+      </c>
+      <c r="O42" t="n">
+        <v>2</v>
+      </c>
+      <c r="P42" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="Q42" t="n">
+        <v>1</v>
+      </c>
+      <c r="R42" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="S42" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T42" t="n">
+        <v>53.95</v>
+      </c>
+      <c r="U42" t="inlineStr">
+        <is>
+          <t>neutral</t>
+        </is>
+      </c>
+      <c r="V42" t="n">
+        <v>0.2767</v>
+      </c>
+      <c r="W42" t="inlineStr">
+        <is>
+          <t>bullish</t>
+        </is>
+      </c>
+      <c r="X42" t="n">
+        <v>-0.014</v>
+      </c>
+      <c r="Y42" t="n">
+        <v>-0.023</v>
+      </c>
+      <c r="Z42" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA42" t="n">
+        <v>59.1</v>
+      </c>
+      <c r="AB42" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC42" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="AD42" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="AE42" t="n">
+        <v>12.26</v>
+      </c>
+      <c r="AF42" t="n">
+        <v>127.64</v>
+      </c>
+      <c r="AG42" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="AH42" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI42" t="n">
+        <v>124.21</v>
+      </c>
+      <c r="AJ42" t="n">
+        <v>125.55</v>
+      </c>
+      <c r="AK42" t="n">
+        <v>124.21</v>
+      </c>
+      <c r="AL42" t="n">
+        <v>0.33</v>
+      </c>
+      <c r="AM42" t="inlineStr">
+        <is>
+          <t>Consider long position</t>
+        </is>
+      </c>
+      <c r="AN42" t="n">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C43" t="n">
+        <v>124.5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>128.34</v>
+      </c>
+      <c r="E43" t="n">
+        <v>124.13</v>
+      </c>
+      <c r="F43" t="n">
+        <v>-2.72</v>
+      </c>
+      <c r="G43" t="n">
+        <v>-2.138</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2027997.9</v>
+      </c>
+      <c r="I43" t="n">
+        <v>256355048.42181</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1076171</v>
+      </c>
+      <c r="K43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="L43" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="M43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="N43" t="n">
+        <v>7</v>
+      </c>
+      <c r="O43" t="n">
+        <v>2</v>
+      </c>
+      <c r="P43" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="Q43" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="R43" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="S43" t="inlineStr">
+        <is>
+          <t>low</t>
+        </is>
+      </c>
+      <c r="T43" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="U43" t="inlineStr">
+        <is>
+          <t>oversold</t>
+        </is>
+      </c>
+      <c r="V43" t="n">
+        <v>-0.377</v>
+      </c>
+      <c r="W43" t="inlineStr">
+        <is>
+          <t>bearish</t>
+        </is>
+      </c>
+      <c r="X43" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="Y43" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="Z43" t="n">
+        <v>0</v>
+      </c>
+      <c r="AA43" t="n">
+        <v>59.2</v>
+      </c>
+      <c r="AB43" t="inlineStr">
+        <is>
+          <t>Neutral</t>
+        </is>
+      </c>
+      <c r="AC43" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="AD43" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="AE43" t="n">
+        <v>7.66</v>
+      </c>
+      <c r="AF43" t="n">
+        <v>125.52</v>
+      </c>
+      <c r="AG43" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="AH43" t="inlineStr">
+        <is>
+          <t>upward</t>
+        </is>
+      </c>
+      <c r="AI43" t="n">
+        <v>124.12</v>
+      </c>
+      <c r="AJ43" t="n">
+        <v>125.7</v>
+      </c>
+      <c r="AK43" t="n">
+        <v>124.12</v>
+      </c>
+      <c r="AL43" t="n">
+        <v>0.17</v>
+      </c>
+      <c r="AM43" t="inlineStr">
+        <is>
+          <t>Hold or wait for clearer signals</t>
+        </is>
+      </c>
+      <c r="AN43" t="n">
+        <v>0.53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
@@ -7030,7 +8272,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H36"/>
+  <dimension ref="A1:H45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8009,6 +9251,258 @@
       </c>
       <c r="H36" t="n">
         <v>3076104.036</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C37" t="n">
+        <v>130.15</v>
+      </c>
+      <c r="D37" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E37" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F37" t="n">
+        <v>2.6</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2.038</v>
+      </c>
+      <c r="H37" t="n">
+        <v>2949879.654</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>130.17</v>
+      </c>
+      <c r="D38" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E38" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F38" t="n">
+        <v>3.31</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2.609</v>
+      </c>
+      <c r="H38" t="n">
+        <v>2904901.346</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C39" t="n">
+        <v>128.12</v>
+      </c>
+      <c r="D39" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E39" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-2.57</v>
+      </c>
+      <c r="G39" t="n">
+        <v>-1.966</v>
+      </c>
+      <c r="H39" t="n">
+        <v>2634025.992</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C40" t="n">
+        <v>127.93</v>
+      </c>
+      <c r="D40" t="n">
+        <v>132.17</v>
+      </c>
+      <c r="E40" t="n">
+        <v>125.26</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.59</v>
+      </c>
+      <c r="H40" t="n">
+        <v>2537841.581</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C41" t="n">
+        <v>128.17</v>
+      </c>
+      <c r="D41" t="n">
+        <v>129.76</v>
+      </c>
+      <c r="E41" t="n">
+        <v>125.28</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.078</v>
+      </c>
+      <c r="H41" t="n">
+        <v>1904825.519</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>120.91</v>
+      </c>
+      <c r="D42" t="n">
+        <v>127.76</v>
+      </c>
+      <c r="E42" t="n">
+        <v>120.44</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-6.38</v>
+      </c>
+      <c r="G42" t="n">
+        <v>-5.012</v>
+      </c>
+      <c r="H42" t="n">
+        <v>2248082.51</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C43" t="n">
+        <v>124.19</v>
+      </c>
+      <c r="D43" t="n">
+        <v>125.6</v>
+      </c>
+      <c r="E43" t="n">
+        <v>121.76</v>
+      </c>
+      <c r="F43" t="n">
+        <v>1.55</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.264</v>
+      </c>
+      <c r="H43" t="n">
+        <v>2052108.573</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C44" t="n">
+        <v>125.15</v>
+      </c>
+      <c r="D44" t="n">
+        <v>126.79</v>
+      </c>
+      <c r="E44" t="n">
+        <v>123.12</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.498</v>
+      </c>
+      <c r="H44" t="n">
+        <v>1788683.963</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C45" t="n">
+        <v>124.5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>128.34</v>
+      </c>
+      <c r="E45" t="n">
+        <v>124.13</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-2.72</v>
+      </c>
+      <c r="G45" t="n">
+        <v>-2.138</v>
+      </c>
+      <c r="H45" t="n">
+        <v>2027997.9</v>
       </c>
     </row>
   </sheetData>
@@ -8023,7 +9517,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8794,6 +10288,204 @@
       </c>
       <c r="F36" t="n">
         <v>0.4808</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>-0.27</v>
+      </c>
+      <c r="E37" t="n">
+        <v>36.63</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.3967</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>-0.11</v>
+      </c>
+      <c r="E38" t="n">
+        <v>44.73</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.3562</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E39" t="n">
+        <v>28.04</v>
+      </c>
+      <c r="F39" t="n">
+        <v>-0.0298</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D40" t="n">
+        <v>-0.36</v>
+      </c>
+      <c r="E40" t="n">
+        <v>32.05</v>
+      </c>
+      <c r="F40" t="n">
+        <v>-0.1863</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C41" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-0.08</v>
+      </c>
+      <c r="E41" t="n">
+        <v>46.15</v>
+      </c>
+      <c r="F41" t="n">
+        <v>-0.3144</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>12.17</v>
+      </c>
+      <c r="F42" t="n">
+        <v>-1.2877</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C43" t="n">
+        <v>1</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.12</v>
+      </c>
+      <c r="E43" t="n">
+        <v>55.79</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.3556</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C44" t="n">
+        <v>1</v>
+      </c>
+      <c r="D44" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="E44" t="n">
+        <v>53.95</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.2767</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>21.62</v>
+      </c>
+      <c r="F45" t="n">
+        <v>-0.377</v>
       </c>
     </row>
   </sheetData>
@@ -8808,7 +10500,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -9682,6 +11374,231 @@
         <v>7</v>
       </c>
       <c r="G36" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C37" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D37" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E37" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F37" t="n">
+        <v>7</v>
+      </c>
+      <c r="G37" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D38" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E38" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F38" t="n">
+        <v>7</v>
+      </c>
+      <c r="G38" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E39" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F39" t="n">
+        <v>7</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D40" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E40" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F40" t="n">
+        <v>7</v>
+      </c>
+      <c r="G40" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F41" t="n">
+        <v>7</v>
+      </c>
+      <c r="G41" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F42" t="n">
+        <v>7</v>
+      </c>
+      <c r="G42" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E43" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F43" t="n">
+        <v>7</v>
+      </c>
+      <c r="G43" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C44" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D44" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E44" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F44" t="n">
+        <v>7</v>
+      </c>
+      <c r="G44" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C45" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="F45" t="n">
+        <v>7</v>
+      </c>
+      <c r="G45" t="n">
         <v>2</v>
       </c>
     </row>
@@ -9697,7 +11614,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -10468,6 +12385,204 @@
       </c>
       <c r="F36" t="n">
         <v>52.4</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C37" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="D37" t="n">
+        <v>0.134</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0</v>
+      </c>
+      <c r="F37" t="n">
+        <v>61.9</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>0.083</v>
+      </c>
+      <c r="D38" t="n">
+        <v>0.138</v>
+      </c>
+      <c r="E38" t="n">
+        <v>0</v>
+      </c>
+      <c r="F38" t="n">
+        <v>62.3</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C39" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="D39" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="E39" t="n">
+        <v>0</v>
+      </c>
+      <c r="F39" t="n">
+        <v>58.3</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C40" t="n">
+        <v>0.046</v>
+      </c>
+      <c r="D40" t="n">
+        <v>0.077</v>
+      </c>
+      <c r="E40" t="n">
+        <v>0</v>
+      </c>
+      <c r="F40" t="n">
+        <v>60.2</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C41" t="n">
+        <v>-0.12</v>
+      </c>
+      <c r="D41" t="n">
+        <v>-0.2</v>
+      </c>
+      <c r="E41" t="n">
+        <v>0</v>
+      </c>
+      <c r="F41" t="n">
+        <v>57.1</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.167</v>
+      </c>
+      <c r="E42" t="n">
+        <v>0</v>
+      </c>
+      <c r="F42" t="n">
+        <v>47.9</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C43" t="n">
+        <v>0.125</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.208</v>
+      </c>
+      <c r="E43" t="n">
+        <v>0</v>
+      </c>
+      <c r="F43" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C44" t="n">
+        <v>-0.014</v>
+      </c>
+      <c r="D44" t="n">
+        <v>-0.023</v>
+      </c>
+      <c r="E44" t="n">
+        <v>0</v>
+      </c>
+      <c r="F44" t="n">
+        <v>59.1</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C45" t="n">
+        <v>0.108</v>
+      </c>
+      <c r="D45" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0</v>
+      </c>
+      <c r="F45" t="n">
+        <v>59.2</v>
       </c>
     </row>
   </sheetData>
@@ -10482,7 +12597,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I36"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -11567,6 +13682,285 @@
         <v>130.65</v>
       </c>
     </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>15:26:03 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B37" s="5" t="n">
+        <v>46044.64309942676</v>
+      </c>
+      <c r="C37" t="n">
+        <v>130.15</v>
+      </c>
+      <c r="D37" t="n">
+        <v>131.44</v>
+      </c>
+      <c r="E37" t="n">
+        <v>0.99</v>
+      </c>
+      <c r="F37" t="n">
+        <v>0.658</v>
+      </c>
+      <c r="G37" t="n">
+        <v>0.342</v>
+      </c>
+      <c r="H37" t="n">
+        <v>129.96</v>
+      </c>
+      <c r="I37" t="n">
+        <v>130.59</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>17:36:52 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B38" s="5" t="n">
+        <v>46044.73394534556</v>
+      </c>
+      <c r="C38" t="n">
+        <v>130.17</v>
+      </c>
+      <c r="D38" t="n">
+        <v>131.81</v>
+      </c>
+      <c r="E38" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F38" t="n">
+        <v>0.5580000000000001</v>
+      </c>
+      <c r="G38" t="n">
+        <v>0.442</v>
+      </c>
+      <c r="H38" t="n">
+        <v>129.83</v>
+      </c>
+      <c r="I38" t="n">
+        <v>130.69</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>20:47:05 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B39" s="5" t="n">
+        <v>46044.86603758115</v>
+      </c>
+      <c r="C39" t="n">
+        <v>128.12</v>
+      </c>
+      <c r="D39" t="n">
+        <v>129.8</v>
+      </c>
+      <c r="E39" t="n">
+        <v>1.31</v>
+      </c>
+      <c r="F39" t="n">
+        <v>0.48</v>
+      </c>
+      <c r="G39" t="n">
+        <v>0.52</v>
+      </c>
+      <c r="H39" t="n">
+        <v>127.33</v>
+      </c>
+      <c r="I39" t="n">
+        <v>128.96</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>22:21:20 22/01/2026</t>
+        </is>
+      </c>
+      <c r="B40" s="5" t="n">
+        <v>46044.9314873316</v>
+      </c>
+      <c r="C40" t="n">
+        <v>127.93</v>
+      </c>
+      <c r="D40" t="n">
+        <v>129.55</v>
+      </c>
+      <c r="E40" t="n">
+        <v>1.27</v>
+      </c>
+      <c r="F40" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="G40" t="n">
+        <v>0.62</v>
+      </c>
+      <c r="H40" t="n">
+        <v>127.87</v>
+      </c>
+      <c r="I40" t="n">
+        <v>128.97</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>22:33:45 23/01/2026</t>
+        </is>
+      </c>
+      <c r="B41" s="5" t="n">
+        <v>46045.94010570139</v>
+      </c>
+      <c r="C41" t="n">
+        <v>128.17</v>
+      </c>
+      <c r="D41" t="n">
+        <v>126.92</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.97</v>
+      </c>
+      <c r="F41" t="n">
+        <v>0.463</v>
+      </c>
+      <c r="G41" t="n">
+        <v>0.537</v>
+      </c>
+      <c r="H41" t="n">
+        <v>127.71</v>
+      </c>
+      <c r="I41" t="n">
+        <v>129.24</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>00:54:26 26/01/2026</t>
+        </is>
+      </c>
+      <c r="B42" s="5" t="n">
+        <v>46048.03781021229</v>
+      </c>
+      <c r="C42" t="n">
+        <v>120.91</v>
+      </c>
+      <c r="D42" t="n">
+        <v>119.22</v>
+      </c>
+      <c r="E42" t="n">
+        <v>-1.4</v>
+      </c>
+      <c r="F42" t="n">
+        <v>0.46</v>
+      </c>
+      <c r="G42" t="n">
+        <v>0.54</v>
+      </c>
+      <c r="H42" t="n">
+        <v>120.85</v>
+      </c>
+      <c r="I42" t="n">
+        <v>122.04</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>10:48:14 27/01/2026</t>
+        </is>
+      </c>
+      <c r="B43" s="5" t="n">
+        <v>46049.45017270291</v>
+      </c>
+      <c r="C43" t="n">
+        <v>124.19</v>
+      </c>
+      <c r="D43" t="n">
+        <v>123.59</v>
+      </c>
+      <c r="E43" t="n">
+        <v>-0.48</v>
+      </c>
+      <c r="F43" t="n">
+        <v>0.662</v>
+      </c>
+      <c r="G43" t="n">
+        <v>0.338</v>
+      </c>
+      <c r="H43" t="n">
+        <v>123.84</v>
+      </c>
+      <c r="I43" t="n">
+        <v>124.97</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>00:19:04 28/01/2026</t>
+        </is>
+      </c>
+      <c r="B44" s="5" t="n">
+        <v>46050.01324256494</v>
+      </c>
+      <c r="C44" t="n">
+        <v>125.15</v>
+      </c>
+      <c r="D44" t="n">
+        <v>127.64</v>
+      </c>
+      <c r="E44" t="n">
+        <v>1.99</v>
+      </c>
+      <c r="F44" t="n">
+        <v>0.649</v>
+      </c>
+      <c r="G44" t="n">
+        <v>0.351</v>
+      </c>
+      <c r="H44" t="n">
+        <v>124.21</v>
+      </c>
+      <c r="I44" t="n">
+        <v>125.55</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>07:58:29 29/01/2026</t>
+        </is>
+      </c>
+      <c r="B45" s="5" t="n">
+        <v>46051.33228866676</v>
+      </c>
+      <c r="C45" t="n">
+        <v>124.5</v>
+      </c>
+      <c r="D45" t="n">
+        <v>125.52</v>
+      </c>
+      <c r="E45" t="n">
+        <v>0.8100000000000001</v>
+      </c>
+      <c r="F45" t="n">
+        <v>0.486</v>
+      </c>
+      <c r="G45" t="n">
+        <v>0.514</v>
+      </c>
+      <c r="H45" t="n">
+        <v>124.12</v>
+      </c>
+      <c r="I45" t="n">
+        <v>125.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <drawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>

</xml_diff>